<commit_message>
24 april 2023 dsr uploading ...
</commit_message>
<xml_diff>
--- a/04_april/AprilDSR.xlsx
+++ b/04_april/AprilDSR.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="94">
   <si>
     <t>Start April Month 2023</t>
   </si>
@@ -227,6 +227,75 @@
   </si>
   <si>
     <t>work on the amount based serching in referral module N check searching is working or not N through the whereq solved</t>
+  </si>
+  <si>
+    <t>update the pr N rebase the pr N check</t>
+  </si>
+  <si>
+    <t>WBX-4494</t>
+  </si>
+  <si>
+    <t>WBX-4487</t>
+  </si>
+  <si>
+    <t>checked box opened textarea in notification if both checked both opened if email checked opened if web checked opened</t>
+  </si>
+  <si>
+    <t>WBX-4493</t>
+  </si>
+  <si>
+    <t>WBX-4453</t>
+  </si>
+  <si>
+    <t>apply translation on add-edit form N referral modules N tracker add edit form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">update the code N raise the pr </t>
+  </si>
+  <si>
+    <t>applied translation on tracker formula add edit N manage tracker module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">applied translation on unit modules N unit- type </t>
+  </si>
+  <si>
+    <t>all hand's meeting with wbx team N binod N sonia</t>
+  </si>
+  <si>
+    <t>applied translation on activity module with create form controls N add placeholder getTranslation</t>
+  </si>
+  <si>
+    <t>update the code N update the pr N rebase the pr</t>
+  </si>
+  <si>
+    <t>applied translation on food modules N special sale details</t>
+  </si>
+  <si>
+    <t>applied translation on user-report module N tracker chart attribute N post module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">applied translation on edit profile N add post module custom error translation N change password </t>
+  </si>
+  <si>
+    <t>R&amp;D for showing preview image orientation in user add edit module</t>
+  </si>
+  <si>
+    <t>WBX-4439</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tried different types of solution N tried them </t>
+  </si>
+  <si>
+    <t>Eid Holiday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">applied translation on login module N update the code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">reviewed pr of harshita </t>
+  </si>
+  <si>
+    <t>applied translation on home module N sign up module</t>
   </si>
 </sst>
 </file>
@@ -234,11 +303,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="dd/mmm/yy"/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="dd/mmm/yy"/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="181" formatCode="h:mm"/>
   </numFmts>
   <fonts count="23">
@@ -281,7 +350,37 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -295,6 +394,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -303,23 +416,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -334,15 +441,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -356,54 +463,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -411,6 +473,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -449,7 +518,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -461,7 +536,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -473,31 +560,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -515,7 +590,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -527,31 +632,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -563,7 +650,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -575,37 +674,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -788,6 +857,48 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -820,9 +931,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -841,199 +954,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1050,7 +1119,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="4" borderId="4" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="4" borderId="4" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="2" fillId="4" borderId="5" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1062,7 +1131,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="4" borderId="7" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="4" borderId="7" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="2" fillId="4" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1074,7 +1143,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="4" borderId="9" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="4" borderId="9" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="2" fillId="4" borderId="10" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1087,7 +1156,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="180" fontId="4" fillId="5" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="5" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1099,7 +1168,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="180" fontId="4" fillId="5" borderId="12" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="5" borderId="12" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="181" fontId="4" fillId="5" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1127,11 +1196,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="180" fontId="4" fillId="5" borderId="12" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="4" fillId="5" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="176" fontId="4" fillId="5" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1452,10 +1518,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A3:N136"/>
+  <dimension ref="A3:N189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="H141" sqref="H141"/>
+    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
+      <selection activeCell="I200" sqref="I200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -3705,80 +3771,1012 @@
       <c r="M130" s="16"/>
       <c r="N130" s="31"/>
     </row>
-    <row r="133" spans="1:14">
-      <c r="A133" s="19" t="s">
+    <row r="134" spans="1:14">
+      <c r="A134" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B134" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C134" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D134" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E134" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F134" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G134" s="18"/>
+      <c r="H134" s="18"/>
+      <c r="I134" s="18"/>
+      <c r="J134" s="18"/>
+      <c r="K134" s="18"/>
+      <c r="L134" s="18"/>
+      <c r="M134" s="18"/>
+      <c r="N134" s="18"/>
+    </row>
+    <row r="135" spans="1:14">
+      <c r="A135" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B133" s="19">
+      <c r="B135" s="19">
         <v>45033</v>
       </c>
-      <c r="C133" s="20"/>
-      <c r="D133" s="21">
+      <c r="C135" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D135" s="21">
         <v>0.385416666666667</v>
       </c>
-      <c r="E133" s="21">
-        <v>0.402777777777778</v>
-      </c>
-      <c r="F133" s="22"/>
-      <c r="G133" s="22"/>
-      <c r="H133" s="22"/>
-      <c r="I133" s="22"/>
-      <c r="J133" s="22"/>
-      <c r="K133" s="22"/>
-      <c r="L133" s="22"/>
-      <c r="M133" s="22"/>
-      <c r="N133" s="22"/>
-    </row>
-    <row r="134" spans="1:14">
-      <c r="A134" s="19"/>
-      <c r="B134" s="19"/>
-      <c r="C134" s="23"/>
-      <c r="D134" s="21"/>
-      <c r="E134" s="21"/>
-      <c r="F134" s="22"/>
-      <c r="G134" s="22"/>
-      <c r="H134" s="22"/>
-      <c r="I134" s="22"/>
-      <c r="J134" s="22"/>
-      <c r="K134" s="22"/>
-      <c r="L134" s="22"/>
-      <c r="M134" s="22"/>
-      <c r="N134" s="22"/>
-    </row>
-    <row r="135" spans="1:14">
-      <c r="A135" s="19"/>
-      <c r="B135" s="19"/>
-      <c r="C135" s="33"/>
-      <c r="D135" s="34"/>
-      <c r="E135" s="34"/>
-      <c r="F135" s="25"/>
-      <c r="G135" s="25"/>
-      <c r="H135" s="25"/>
-      <c r="I135" s="25"/>
-      <c r="J135" s="25"/>
-      <c r="K135" s="25"/>
-      <c r="L135" s="25"/>
-      <c r="M135" s="25"/>
-      <c r="N135" s="25"/>
+      <c r="E135" s="21">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="F135" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G135" s="22"/>
+      <c r="H135" s="22"/>
+      <c r="I135" s="22"/>
+      <c r="J135" s="22"/>
+      <c r="K135" s="22"/>
+      <c r="L135" s="22"/>
+      <c r="M135" s="22"/>
+      <c r="N135" s="22"/>
     </row>
     <row r="136" spans="1:14">
       <c r="A136" s="19"/>
       <c r="B136" s="19"/>
-      <c r="C136" s="33"/>
-      <c r="D136" s="34"/>
-      <c r="E136" s="34"/>
-      <c r="F136" s="25"/>
-      <c r="G136" s="25"/>
-      <c r="H136" s="25"/>
-      <c r="I136" s="25"/>
-      <c r="J136" s="25"/>
-      <c r="K136" s="25"/>
-      <c r="L136" s="25"/>
-      <c r="M136" s="25"/>
-      <c r="N136" s="25"/>
+      <c r="C136" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D136" s="21">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E136" s="21">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="F136" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G136" s="22"/>
+      <c r="H136" s="22"/>
+      <c r="I136" s="22"/>
+      <c r="J136" s="22"/>
+      <c r="K136" s="22"/>
+      <c r="L136" s="22"/>
+      <c r="M136" s="22"/>
+      <c r="N136" s="22"/>
+    </row>
+    <row r="137" spans="1:14">
+      <c r="A137" s="19"/>
+      <c r="B137" s="19"/>
+      <c r="C137" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="D137" s="24">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="E137" s="24">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F137" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="G137" s="25"/>
+      <c r="H137" s="25"/>
+      <c r="I137" s="25"/>
+      <c r="J137" s="25"/>
+      <c r="K137" s="25"/>
+      <c r="L137" s="25"/>
+      <c r="M137" s="25"/>
+      <c r="N137" s="25"/>
+    </row>
+    <row r="138" spans="1:14">
+      <c r="A138" s="19"/>
+      <c r="B138" s="19"/>
+      <c r="C138" s="23"/>
+      <c r="D138" s="24"/>
+      <c r="E138" s="24"/>
+      <c r="F138" s="25"/>
+      <c r="G138" s="25"/>
+      <c r="H138" s="25"/>
+      <c r="I138" s="25"/>
+      <c r="J138" s="25"/>
+      <c r="K138" s="25"/>
+      <c r="L138" s="25"/>
+      <c r="M138" s="25"/>
+      <c r="N138" s="25"/>
+    </row>
+    <row r="139" spans="1:14">
+      <c r="A139" s="19"/>
+      <c r="B139" s="19"/>
+      <c r="C139" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D139" s="21">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E139" s="21">
+        <v>0.09375</v>
+      </c>
+      <c r="F139" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="G139" s="25"/>
+      <c r="H139" s="25"/>
+      <c r="I139" s="25"/>
+      <c r="J139" s="25"/>
+      <c r="K139" s="25"/>
+      <c r="L139" s="25"/>
+      <c r="M139" s="25"/>
+      <c r="N139" s="25"/>
+    </row>
+    <row r="140" spans="1:14">
+      <c r="A140" s="19"/>
+      <c r="B140" s="19"/>
+      <c r="C140" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D140" s="21">
+        <v>0.09375</v>
+      </c>
+      <c r="E140" s="21">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F140" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="G140" s="25"/>
+      <c r="H140" s="25"/>
+      <c r="I140" s="25"/>
+      <c r="J140" s="25"/>
+      <c r="K140" s="25"/>
+      <c r="L140" s="25"/>
+      <c r="M140" s="25"/>
+      <c r="N140" s="25"/>
+    </row>
+    <row r="143" spans="1:14">
+      <c r="A143" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B143" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C143" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D143" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E143" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F143" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G143" s="18"/>
+      <c r="H143" s="18"/>
+      <c r="I143" s="18"/>
+      <c r="J143" s="18"/>
+      <c r="K143" s="18"/>
+      <c r="L143" s="18"/>
+      <c r="M143" s="18"/>
+      <c r="N143" s="18"/>
+    </row>
+    <row r="144" spans="1:14">
+      <c r="A144" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B144" s="19">
+        <v>45034</v>
+      </c>
+      <c r="C144" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D144" s="21">
+        <v>0.388888888888889</v>
+      </c>
+      <c r="E144" s="21">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="F144" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G144" s="22"/>
+      <c r="H144" s="22"/>
+      <c r="I144" s="22"/>
+      <c r="J144" s="22"/>
+      <c r="K144" s="22"/>
+      <c r="L144" s="22"/>
+      <c r="M144" s="22"/>
+      <c r="N144" s="22"/>
+    </row>
+    <row r="145" spans="1:14">
+      <c r="A145" s="19"/>
+      <c r="B145" s="19"/>
+      <c r="C145" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D145" s="21">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E145" s="21">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="F145" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G145" s="22"/>
+      <c r="H145" s="22"/>
+      <c r="I145" s="22"/>
+      <c r="J145" s="22"/>
+      <c r="K145" s="22"/>
+      <c r="L145" s="22"/>
+      <c r="M145" s="22"/>
+      <c r="N145" s="22"/>
+    </row>
+    <row r="146" spans="1:14">
+      <c r="A146" s="19"/>
+      <c r="B146" s="19"/>
+      <c r="C146" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D146" s="21">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="E146" s="21">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F146" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="G146" s="22"/>
+      <c r="H146" s="22"/>
+      <c r="I146" s="22"/>
+      <c r="J146" s="22"/>
+      <c r="K146" s="22"/>
+      <c r="L146" s="22"/>
+      <c r="M146" s="22"/>
+      <c r="N146" s="22"/>
+    </row>
+    <row r="147" spans="1:14">
+      <c r="A147" s="19"/>
+      <c r="B147" s="19"/>
+      <c r="C147" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D147" s="24">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E147" s="24">
+        <v>0.229166666666667</v>
+      </c>
+      <c r="F147" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="G147" s="25"/>
+      <c r="H147" s="25"/>
+      <c r="I147" s="25"/>
+      <c r="J147" s="25"/>
+      <c r="K147" s="25"/>
+      <c r="L147" s="25"/>
+      <c r="M147" s="25"/>
+      <c r="N147" s="25"/>
+    </row>
+    <row r="148" spans="1:14">
+      <c r="A148" s="19"/>
+      <c r="B148" s="19"/>
+      <c r="C148" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D148" s="24">
+        <v>0.229166666666667</v>
+      </c>
+      <c r="E148" s="24">
+        <v>0.25</v>
+      </c>
+      <c r="F148" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="G148" s="25"/>
+      <c r="H148" s="25"/>
+      <c r="I148" s="25"/>
+      <c r="J148" s="25"/>
+      <c r="K148" s="25"/>
+      <c r="L148" s="25"/>
+      <c r="M148" s="25"/>
+      <c r="N148" s="25"/>
+    </row>
+    <row r="149" spans="1:14">
+      <c r="A149" s="19"/>
+      <c r="B149" s="19"/>
+      <c r="C149" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D149" s="24">
+        <v>0.25</v>
+      </c>
+      <c r="E149" s="21">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F149" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="G149" s="25"/>
+      <c r="H149" s="25"/>
+      <c r="I149" s="25"/>
+      <c r="J149" s="25"/>
+      <c r="K149" s="25"/>
+      <c r="L149" s="25"/>
+      <c r="M149" s="25"/>
+      <c r="N149" s="25"/>
+    </row>
+    <row r="152" spans="1:14">
+      <c r="A152" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B152" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C152" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D152" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E152" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F152" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G152" s="18"/>
+      <c r="H152" s="18"/>
+      <c r="I152" s="18"/>
+      <c r="J152" s="18"/>
+      <c r="K152" s="18"/>
+      <c r="L152" s="18"/>
+      <c r="M152" s="18"/>
+      <c r="N152" s="18"/>
+    </row>
+    <row r="153" spans="1:14">
+      <c r="A153" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B153" s="19">
+        <v>45035</v>
+      </c>
+      <c r="C153" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D153" s="21">
+        <v>0.388888888888889</v>
+      </c>
+      <c r="E153" s="21">
+        <v>0.40625</v>
+      </c>
+      <c r="F153" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="G153" s="22"/>
+      <c r="H153" s="22"/>
+      <c r="I153" s="22"/>
+      <c r="J153" s="22"/>
+      <c r="K153" s="22"/>
+      <c r="L153" s="22"/>
+      <c r="M153" s="22"/>
+      <c r="N153" s="22"/>
+    </row>
+    <row r="154" spans="1:14">
+      <c r="A154" s="19"/>
+      <c r="B154" s="19"/>
+      <c r="C154" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D154" s="21">
+        <v>0.40625</v>
+      </c>
+      <c r="E154" s="21">
+        <v>0.413194444444444</v>
+      </c>
+      <c r="F154" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G154" s="22"/>
+      <c r="H154" s="22"/>
+      <c r="I154" s="22"/>
+      <c r="J154" s="22"/>
+      <c r="K154" s="22"/>
+      <c r="L154" s="22"/>
+      <c r="M154" s="22"/>
+      <c r="N154" s="22"/>
+    </row>
+    <row r="155" spans="1:14">
+      <c r="A155" s="19"/>
+      <c r="B155" s="19"/>
+      <c r="C155" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D155" s="21">
+        <v>0.413194444444444</v>
+      </c>
+      <c r="E155" s="21">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F155" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="G155" s="25"/>
+      <c r="H155" s="25"/>
+      <c r="I155" s="25"/>
+      <c r="J155" s="25"/>
+      <c r="K155" s="25"/>
+      <c r="L155" s="25"/>
+      <c r="M155" s="25"/>
+      <c r="N155" s="25"/>
+    </row>
+    <row r="156" spans="1:14">
+      <c r="A156" s="19"/>
+      <c r="B156" s="19"/>
+      <c r="C156" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D156" s="24">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E156" s="24">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F156" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="G156" s="25"/>
+      <c r="H156" s="25"/>
+      <c r="I156" s="25"/>
+      <c r="J156" s="25"/>
+      <c r="K156" s="25"/>
+      <c r="L156" s="25"/>
+      <c r="M156" s="25"/>
+      <c r="N156" s="25"/>
+    </row>
+    <row r="157" spans="1:14">
+      <c r="A157" s="19"/>
+      <c r="B157" s="19"/>
+      <c r="C157" s="23"/>
+      <c r="D157" s="24"/>
+      <c r="E157" s="24"/>
+      <c r="F157" s="25"/>
+      <c r="G157" s="25"/>
+      <c r="H157" s="25"/>
+      <c r="I157" s="25"/>
+      <c r="J157" s="25"/>
+      <c r="K157" s="25"/>
+      <c r="L157" s="25"/>
+      <c r="M157" s="25"/>
+      <c r="N157" s="25"/>
+    </row>
+    <row r="160" spans="1:14">
+      <c r="A160" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B160" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C160" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D160" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E160" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F160" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G160" s="18"/>
+      <c r="H160" s="18"/>
+      <c r="I160" s="18"/>
+      <c r="J160" s="18"/>
+      <c r="K160" s="18"/>
+      <c r="L160" s="18"/>
+      <c r="M160" s="18"/>
+      <c r="N160" s="18"/>
+    </row>
+    <row r="161" spans="1:14">
+      <c r="A161" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B161" s="19">
+        <v>45036</v>
+      </c>
+      <c r="C161" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D161" s="21">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E161" s="21">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="F161" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G161" s="22"/>
+      <c r="H161" s="22"/>
+      <c r="I161" s="22"/>
+      <c r="J161" s="22"/>
+      <c r="K161" s="22"/>
+      <c r="L161" s="22"/>
+      <c r="M161" s="22"/>
+      <c r="N161" s="22"/>
+    </row>
+    <row r="162" spans="1:14">
+      <c r="A162" s="19"/>
+      <c r="B162" s="19"/>
+      <c r="C162" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D162" s="21">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="E162" s="21">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F162" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G162" s="22"/>
+      <c r="H162" s="22"/>
+      <c r="I162" s="22"/>
+      <c r="J162" s="22"/>
+      <c r="K162" s="22"/>
+      <c r="L162" s="22"/>
+      <c r="M162" s="22"/>
+      <c r="N162" s="22"/>
+    </row>
+    <row r="163" spans="1:14">
+      <c r="A163" s="19"/>
+      <c r="B163" s="19"/>
+      <c r="C163" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D163" s="24">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E163" s="24">
+        <v>0.208333333333333</v>
+      </c>
+      <c r="F163" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="G163" s="25"/>
+      <c r="H163" s="25"/>
+      <c r="I163" s="25"/>
+      <c r="J163" s="25"/>
+      <c r="K163" s="25"/>
+      <c r="L163" s="25"/>
+      <c r="M163" s="25"/>
+      <c r="N163" s="25"/>
+    </row>
+    <row r="164" spans="1:14">
+      <c r="A164" s="19"/>
+      <c r="B164" s="19"/>
+      <c r="C164" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="D164" s="24">
+        <v>0.208333333333333</v>
+      </c>
+      <c r="E164" s="24">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F164" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="G164" s="25"/>
+      <c r="H164" s="25"/>
+      <c r="I164" s="25"/>
+      <c r="J164" s="25"/>
+      <c r="K164" s="25"/>
+      <c r="L164" s="25"/>
+      <c r="M164" s="25"/>
+      <c r="N164" s="25"/>
+    </row>
+    <row r="167" spans="1:14">
+      <c r="A167" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D167" s="4"/>
+      <c r="E167" s="4"/>
+      <c r="F167" s="4"/>
+      <c r="G167" s="4"/>
+      <c r="H167" s="4"/>
+      <c r="I167" s="4"/>
+      <c r="J167" s="4"/>
+      <c r="K167" s="4"/>
+      <c r="L167" s="4"/>
+      <c r="M167" s="4"/>
+      <c r="N167" s="28"/>
+    </row>
+    <row r="168" spans="1:14">
+      <c r="A168" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B168" s="6">
+        <v>45037</v>
+      </c>
+      <c r="C168" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D168" s="8"/>
+      <c r="E168" s="8"/>
+      <c r="F168" s="8"/>
+      <c r="G168" s="8"/>
+      <c r="H168" s="8"/>
+      <c r="I168" s="8"/>
+      <c r="J168" s="8"/>
+      <c r="K168" s="8"/>
+      <c r="L168" s="8"/>
+      <c r="M168" s="8"/>
+      <c r="N168" s="29"/>
+    </row>
+    <row r="169" spans="1:14">
+      <c r="A169" s="9"/>
+      <c r="B169" s="10"/>
+      <c r="C169" s="11"/>
+      <c r="D169" s="12"/>
+      <c r="E169" s="12"/>
+      <c r="F169" s="12"/>
+      <c r="G169" s="12"/>
+      <c r="H169" s="12"/>
+      <c r="I169" s="12"/>
+      <c r="J169" s="12"/>
+      <c r="K169" s="12"/>
+      <c r="L169" s="12"/>
+      <c r="M169" s="12"/>
+      <c r="N169" s="30"/>
+    </row>
+    <row r="170" spans="1:14">
+      <c r="A170" s="13"/>
+      <c r="B170" s="14"/>
+      <c r="C170" s="15"/>
+      <c r="D170" s="16"/>
+      <c r="E170" s="16"/>
+      <c r="F170" s="16"/>
+      <c r="G170" s="16"/>
+      <c r="H170" s="16"/>
+      <c r="I170" s="16"/>
+      <c r="J170" s="16"/>
+      <c r="K170" s="16"/>
+      <c r="L170" s="16"/>
+      <c r="M170" s="16"/>
+      <c r="N170" s="31"/>
+    </row>
+    <row r="173" spans="1:14">
+      <c r="A173" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D173" s="4"/>
+      <c r="E173" s="4"/>
+      <c r="F173" s="4"/>
+      <c r="G173" s="4"/>
+      <c r="H173" s="4"/>
+      <c r="I173" s="4"/>
+      <c r="J173" s="4"/>
+      <c r="K173" s="4"/>
+      <c r="L173" s="4"/>
+      <c r="M173" s="4"/>
+      <c r="N173" s="28"/>
+    </row>
+    <row r="174" spans="1:14">
+      <c r="A174" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B174" s="6">
+        <v>45038</v>
+      </c>
+      <c r="C174" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D174" s="8"/>
+      <c r="E174" s="8"/>
+      <c r="F174" s="8"/>
+      <c r="G174" s="8"/>
+      <c r="H174" s="8"/>
+      <c r="I174" s="8"/>
+      <c r="J174" s="8"/>
+      <c r="K174" s="8"/>
+      <c r="L174" s="8"/>
+      <c r="M174" s="8"/>
+      <c r="N174" s="29"/>
+    </row>
+    <row r="175" spans="1:14">
+      <c r="A175" s="9"/>
+      <c r="B175" s="10"/>
+      <c r="C175" s="11"/>
+      <c r="D175" s="12"/>
+      <c r="E175" s="12"/>
+      <c r="F175" s="12"/>
+      <c r="G175" s="12"/>
+      <c r="H175" s="12"/>
+      <c r="I175" s="12"/>
+      <c r="J175" s="12"/>
+      <c r="K175" s="12"/>
+      <c r="L175" s="12"/>
+      <c r="M175" s="12"/>
+      <c r="N175" s="30"/>
+    </row>
+    <row r="176" spans="1:14">
+      <c r="A176" s="13"/>
+      <c r="B176" s="14"/>
+      <c r="C176" s="15"/>
+      <c r="D176" s="16"/>
+      <c r="E176" s="16"/>
+      <c r="F176" s="16"/>
+      <c r="G176" s="16"/>
+      <c r="H176" s="16"/>
+      <c r="I176" s="16"/>
+      <c r="J176" s="16"/>
+      <c r="K176" s="16"/>
+      <c r="L176" s="16"/>
+      <c r="M176" s="16"/>
+      <c r="N176" s="31"/>
+    </row>
+    <row r="177" spans="1:14">
+      <c r="A177" s="17"/>
+      <c r="B177" s="17"/>
+      <c r="C177" s="17"/>
+      <c r="D177" s="17"/>
+      <c r="E177" s="17"/>
+      <c r="F177" s="17"/>
+      <c r="G177" s="17"/>
+      <c r="H177" s="17"/>
+      <c r="I177" s="17"/>
+      <c r="J177" s="17"/>
+      <c r="K177" s="17"/>
+      <c r="L177" s="17"/>
+      <c r="M177" s="17"/>
+      <c r="N177" s="17"/>
+    </row>
+    <row r="178" spans="1:14">
+      <c r="A178" s="17"/>
+      <c r="B178" s="17"/>
+      <c r="C178" s="17"/>
+      <c r="D178" s="17"/>
+      <c r="E178" s="17"/>
+      <c r="F178" s="17"/>
+      <c r="G178" s="17"/>
+      <c r="H178" s="17"/>
+      <c r="I178" s="17"/>
+      <c r="J178" s="17"/>
+      <c r="K178" s="17"/>
+      <c r="L178" s="17"/>
+      <c r="M178" s="17"/>
+      <c r="N178" s="17"/>
+    </row>
+    <row r="179" spans="1:14">
+      <c r="A179" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D179" s="4"/>
+      <c r="E179" s="4"/>
+      <c r="F179" s="4"/>
+      <c r="G179" s="4"/>
+      <c r="H179" s="4"/>
+      <c r="I179" s="4"/>
+      <c r="J179" s="4"/>
+      <c r="K179" s="4"/>
+      <c r="L179" s="4"/>
+      <c r="M179" s="4"/>
+      <c r="N179" s="28"/>
+    </row>
+    <row r="180" spans="1:14">
+      <c r="A180" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B180" s="6">
+        <v>45039</v>
+      </c>
+      <c r="C180" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D180" s="8"/>
+      <c r="E180" s="8"/>
+      <c r="F180" s="8"/>
+      <c r="G180" s="8"/>
+      <c r="H180" s="8"/>
+      <c r="I180" s="8"/>
+      <c r="J180" s="8"/>
+      <c r="K180" s="8"/>
+      <c r="L180" s="8"/>
+      <c r="M180" s="8"/>
+      <c r="N180" s="29"/>
+    </row>
+    <row r="181" spans="1:14">
+      <c r="A181" s="9"/>
+      <c r="B181" s="10"/>
+      <c r="C181" s="11"/>
+      <c r="D181" s="12"/>
+      <c r="E181" s="12"/>
+      <c r="F181" s="12"/>
+      <c r="G181" s="12"/>
+      <c r="H181" s="12"/>
+      <c r="I181" s="12"/>
+      <c r="J181" s="12"/>
+      <c r="K181" s="12"/>
+      <c r="L181" s="12"/>
+      <c r="M181" s="12"/>
+      <c r="N181" s="30"/>
+    </row>
+    <row r="182" spans="1:14">
+      <c r="A182" s="13"/>
+      <c r="B182" s="14"/>
+      <c r="C182" s="15"/>
+      <c r="D182" s="16"/>
+      <c r="E182" s="16"/>
+      <c r="F182" s="16"/>
+      <c r="G182" s="16"/>
+      <c r="H182" s="16"/>
+      <c r="I182" s="16"/>
+      <c r="J182" s="16"/>
+      <c r="K182" s="16"/>
+      <c r="L182" s="16"/>
+      <c r="M182" s="16"/>
+      <c r="N182" s="31"/>
+    </row>
+    <row r="185" spans="1:14">
+      <c r="A185" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B185" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C185" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D185" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E185" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F185" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G185" s="18"/>
+      <c r="H185" s="18"/>
+      <c r="I185" s="18"/>
+      <c r="J185" s="18"/>
+      <c r="K185" s="18"/>
+      <c r="L185" s="18"/>
+      <c r="M185" s="18"/>
+      <c r="N185" s="18"/>
+    </row>
+    <row r="186" spans="1:14">
+      <c r="A186" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B186" s="19">
+        <v>45040</v>
+      </c>
+      <c r="C186" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D186" s="21">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E186" s="21">
+        <v>0.399305555555556</v>
+      </c>
+      <c r="F186" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G186" s="22"/>
+      <c r="H186" s="22"/>
+      <c r="I186" s="22"/>
+      <c r="J186" s="22"/>
+      <c r="K186" s="22"/>
+      <c r="L186" s="22"/>
+      <c r="M186" s="22"/>
+      <c r="N186" s="22"/>
+    </row>
+    <row r="187" spans="1:14">
+      <c r="A187" s="19"/>
+      <c r="B187" s="19"/>
+      <c r="C187" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D187" s="21">
+        <v>0.399305555555556</v>
+      </c>
+      <c r="E187" s="21">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F187" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="G187" s="22"/>
+      <c r="H187" s="22"/>
+      <c r="I187" s="22"/>
+      <c r="J187" s="22"/>
+      <c r="K187" s="22"/>
+      <c r="L187" s="22"/>
+      <c r="M187" s="22"/>
+      <c r="N187" s="22"/>
+    </row>
+    <row r="188" spans="1:14">
+      <c r="A188" s="19"/>
+      <c r="B188" s="19"/>
+      <c r="C188" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D188" s="21">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E188" s="24">
+        <v>0.09375</v>
+      </c>
+      <c r="F188" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G188" s="25"/>
+      <c r="H188" s="25"/>
+      <c r="I188" s="25"/>
+      <c r="J188" s="25"/>
+      <c r="K188" s="25"/>
+      <c r="L188" s="25"/>
+      <c r="M188" s="25"/>
+      <c r="N188" s="25"/>
+    </row>
+    <row r="189" spans="1:14">
+      <c r="A189" s="33"/>
+      <c r="B189" s="33"/>
+      <c r="C189" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D189" s="24">
+        <v>0.09375</v>
+      </c>
+      <c r="E189" s="24">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F189" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="G189" s="25"/>
+      <c r="H189" s="25"/>
+      <c r="I189" s="25"/>
+      <c r="J189" s="25"/>
+      <c r="K189" s="25"/>
+      <c r="L189" s="25"/>
+      <c r="M189" s="25"/>
+      <c r="N189" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="140">
+  <mergeCells count="190">
     <mergeCell ref="C8:N8"/>
     <mergeCell ref="C14:N14"/>
     <mergeCell ref="F20:N20"/>
@@ -3834,10 +4832,35 @@
     <mergeCell ref="F121:N121"/>
     <mergeCell ref="F122:N122"/>
     <mergeCell ref="C127:N127"/>
-    <mergeCell ref="F133:N133"/>
     <mergeCell ref="F134:N134"/>
     <mergeCell ref="F135:N135"/>
     <mergeCell ref="F136:N136"/>
+    <mergeCell ref="F139:N139"/>
+    <mergeCell ref="F140:N140"/>
+    <mergeCell ref="F143:N143"/>
+    <mergeCell ref="F144:N144"/>
+    <mergeCell ref="F145:N145"/>
+    <mergeCell ref="F146:N146"/>
+    <mergeCell ref="F147:N147"/>
+    <mergeCell ref="F148:N148"/>
+    <mergeCell ref="F149:N149"/>
+    <mergeCell ref="F152:N152"/>
+    <mergeCell ref="F153:N153"/>
+    <mergeCell ref="F154:N154"/>
+    <mergeCell ref="F155:N155"/>
+    <mergeCell ref="F160:N160"/>
+    <mergeCell ref="F161:N161"/>
+    <mergeCell ref="F162:N162"/>
+    <mergeCell ref="F163:N163"/>
+    <mergeCell ref="F164:N164"/>
+    <mergeCell ref="C167:N167"/>
+    <mergeCell ref="C173:N173"/>
+    <mergeCell ref="C179:N179"/>
+    <mergeCell ref="F185:N185"/>
+    <mergeCell ref="F186:N186"/>
+    <mergeCell ref="F187:N187"/>
+    <mergeCell ref="F188:N188"/>
+    <mergeCell ref="F189:N189"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A21:A24"/>
@@ -3854,7 +4877,14 @@
     <mergeCell ref="A115:A117"/>
     <mergeCell ref="A121:A124"/>
     <mergeCell ref="A128:A130"/>
-    <mergeCell ref="A133:A136"/>
+    <mergeCell ref="A135:A140"/>
+    <mergeCell ref="A144:A149"/>
+    <mergeCell ref="A153:A157"/>
+    <mergeCell ref="A161:A164"/>
+    <mergeCell ref="A168:A170"/>
+    <mergeCell ref="A174:A176"/>
+    <mergeCell ref="A180:A182"/>
+    <mergeCell ref="A186:A189"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="B21:B24"/>
@@ -3871,7 +4901,14 @@
     <mergeCell ref="B115:B117"/>
     <mergeCell ref="B121:B124"/>
     <mergeCell ref="B128:B130"/>
-    <mergeCell ref="B133:B136"/>
+    <mergeCell ref="B135:B140"/>
+    <mergeCell ref="B144:B149"/>
+    <mergeCell ref="B153:B157"/>
+    <mergeCell ref="B161:B164"/>
+    <mergeCell ref="B168:B170"/>
+    <mergeCell ref="B174:B176"/>
+    <mergeCell ref="B180:B182"/>
+    <mergeCell ref="B186:B189"/>
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="C30:C31"/>
     <mergeCell ref="C33:C34"/>
@@ -3882,6 +4919,8 @@
     <mergeCell ref="C102:C103"/>
     <mergeCell ref="C110:C111"/>
     <mergeCell ref="C123:C124"/>
+    <mergeCell ref="C137:C138"/>
+    <mergeCell ref="C156:C157"/>
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="D30:D31"/>
     <mergeCell ref="D33:D34"/>
@@ -3892,6 +4931,8 @@
     <mergeCell ref="D102:D103"/>
     <mergeCell ref="D110:D111"/>
     <mergeCell ref="D123:D124"/>
+    <mergeCell ref="D137:D138"/>
+    <mergeCell ref="D156:D157"/>
     <mergeCell ref="E23:E24"/>
     <mergeCell ref="E30:E31"/>
     <mergeCell ref="E33:E34"/>
@@ -3902,6 +4943,8 @@
     <mergeCell ref="E102:E103"/>
     <mergeCell ref="E110:E111"/>
     <mergeCell ref="E123:E124"/>
+    <mergeCell ref="E137:E138"/>
+    <mergeCell ref="E156:E157"/>
     <mergeCell ref="D3:K4"/>
     <mergeCell ref="C9:N11"/>
     <mergeCell ref="C15:N17"/>
@@ -3919,6 +4962,11 @@
     <mergeCell ref="C115:N117"/>
     <mergeCell ref="F123:N124"/>
     <mergeCell ref="C128:N130"/>
+    <mergeCell ref="F137:N138"/>
+    <mergeCell ref="F156:N157"/>
+    <mergeCell ref="C168:N170"/>
+    <mergeCell ref="C174:N176"/>
+    <mergeCell ref="C180:N182"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>